<commit_message>
updated folders, working on ortholinear A* aglorithm
</commit_message>
<xml_diff>
--- a/adjacentMatrix.xlsx
+++ b/adjacentMatrix.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Programming/Personal_Projects/Adjacent_letters_in_names/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthenderson/Documents/z-Practice/Github/adjacentLetters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455D84C2-FD31-0E48-9B25-3803F9D16BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83836F09-3AEC-C244-93C5-1C49A85CACC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{B156F02B-E409-A541-969B-D4278EA2A925}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="31800" windowHeight="19860" activeTab="1" xr2:uid="{B156F02B-E409-A541-969B-D4278EA2A925}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Qwerty" sheetId="1" r:id="rId1"/>
+    <sheet name="OrthoLinear" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -113,6 +105,9 @@
   <si>
     <t>Z</t>
   </si>
+  <si>
+    <t>SUM</t>
+  </si>
 </sst>
 </file>
 
@@ -149,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,11 +167,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -190,11 +196,37 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -527,9 +559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82C641D-1E4C-5D43-B403-218CDC5CBC11}">
   <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD19" sqref="AD19"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2780,14 +2812,1307 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AA27">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61141074-5654-9640-8A2F-A28250876D5F}">
+  <dimension ref="A1:AB27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC35" sqref="AC35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="2.33203125" customWidth="1"/>
+    <col min="28" max="28" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="8">
+        <f>COUNT(B2:AA2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="8">
+        <f t="shared" ref="AB3:AB27" si="0">COUNT(B3:AA3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2">
+        <v>1</v>
+      </c>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2">
+        <v>1</v>
+      </c>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2">
+        <v>1</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2">
+        <v>1</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2">
+        <v>1</v>
+      </c>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2">
+        <v>1</v>
+      </c>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2">
+        <v>1</v>
+      </c>
+      <c r="V26" s="2">
+        <v>1</v>
+      </c>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:AA27">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>